<commit_message>
Proyecto final parte 1 completado
</commit_message>
<xml_diff>
--- a/Proyecto Final/Variables.xlsx
+++ b/Proyecto Final/Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joran\Desktop\Maestría en Ciencia de Datos\Análisis exploratorio de datos\Proyecto Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F48A9D-2FE4-4E43-93D3-5994DAEC5D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4739E1A-CB79-4863-B6C5-5DD037A5374F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{61A84A6B-FC75-4228-96B4-3E6CEAA5F620}"/>
   </bookViews>
@@ -533,7 +533,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C3" sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>